<commit_message>
Added tooltip to map + added description to county names
</commit_message>
<xml_diff>
--- a/data/interim/unemployment.xlsx
+++ b/data/interim/unemployment.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>bolesławiecki</t>
+          <t>powiat bolesławiecki</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dzierżoniowski</t>
+          <t>powiat dzierżoniowski</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -534,7 +534,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>głogowski</t>
+          <t>powiat głogowski</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -562,7 +562,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>górowski</t>
+          <t>powiat górowski</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -590,7 +590,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>jaworski</t>
+          <t>powiat jaworski</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -618,7 +618,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>karkonoski</t>
+          <t>powiat karkonoski</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>kamiennogórski</t>
+          <t>powiat kamiennogórski</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -674,7 +674,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>kłodzki</t>
+          <t>powiat kłodzki</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -702,7 +702,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>legnicki</t>
+          <t>powiat legnicki</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -728,7 +728,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>lubański</t>
+          <t>powiat lubański</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -754,7 +754,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>lubiński</t>
+          <t>powiat lubiński</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -780,7 +780,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lwówecki</t>
+          <t>powiat lwówecki</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>milicki</t>
+          <t>powiat milicki</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -832,7 +832,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>oleśnicki</t>
+          <t>powiat oleśnicki</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -858,7 +858,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>oławski</t>
+          <t>powiat oławski</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -884,7 +884,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>polkowicki</t>
+          <t>powiat polkowicki</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>strzeliński</t>
+          <t>powiat strzeliński</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -936,7 +936,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>średzki</t>
+          <t>powiat średzki</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -962,7 +962,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>świdnicki</t>
+          <t>powiat świdnicki</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>trzebnicki</t>
+          <t>powiat trzebnicki</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>wałbrzyski</t>
+          <t>powiat wałbrzyski</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>wołowski</t>
+          <t>powiat wołowski</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>wrocławski</t>
+          <t>powiat wrocławski</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ząbkowicki</t>
+          <t>powiat ząbkowicki</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>zgorzelecki</t>
+          <t>powiat zgorzelecki</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>złotoryjski</t>
+          <t>powiat złotoryjski</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>m.JeleniaGóra</t>
+          <t>miasto JeleniaGóra</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>m.Legnica</t>
+          <t>miasto Legnica</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>m.Wrocław</t>
+          <t>miasto Wrocław</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>m.Wałbrzych</t>
+          <t>miasto Wałbrzych</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>aleksandrowski</t>
+          <t>powiat aleksandrowski</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>brodnicki</t>
+          <t>powiat brodnicki</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>bydgoski</t>
+          <t>powiat bydgoski</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>chełmiński</t>
+          <t>powiat chełmiński</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>golubsko-dobrzyński</t>
+          <t>powiat golubsko-dobrzyński</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>grudziądzki</t>
+          <t>powiat grudziądzki</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>inowrocławski</t>
+          <t>powiat inowrocławski</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>lipnowski</t>
+          <t>powiat lipnowski</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>mogileński</t>
+          <t>powiat mogileński</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>nakielski</t>
+          <t>powiat nakielski</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>radziejowski</t>
+          <t>powiat radziejowski</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>rypiński</t>
+          <t>powiat rypiński</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>sępoleński</t>
+          <t>powiat sępoleński</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>świecki</t>
+          <t>powiat świecki</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>toruński</t>
+          <t>powiat toruński</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>tucholski</t>
+          <t>powiat tucholski</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>wąbrzeski</t>
+          <t>powiat wąbrzeski</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>włocławski</t>
+          <t>powiat włocławski</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>żniński</t>
+          <t>powiat żniński</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>m.Bydgoszcz</t>
+          <t>miasto Bydgoszcz</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>m.Grudziądz</t>
+          <t>miasto Grudziądz</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>m.Toruń</t>
+          <t>miasto Toruń</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>m.Włocławek</t>
+          <t>miasto Włocławek</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>bialski</t>
+          <t>powiat bialski</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>biłgorajski</t>
+          <t>powiat biłgorajski</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>chełmski</t>
+          <t>powiat chełmski</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>hrubieszowski</t>
+          <t>powiat hrubieszowski</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -2004,7 +2004,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>janowski</t>
+          <t>powiat janowski</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>krasnostawski</t>
+          <t>powiat krasnostawski</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>kraśnicki</t>
+          <t>powiat kraśnicki</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>lubartowski</t>
+          <t>powiat lubartowski</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>lubelski</t>
+          <t>powiat lubelski</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>łęczyński</t>
+          <t>powiat łęczyński</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>łukowski</t>
+          <t>powiat łukowski</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>opolski</t>
+          <t>powiat opolski</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>parczewski</t>
+          <t>powiat parczewski</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>puławski</t>
+          <t>powiat puławski</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>radzyński</t>
+          <t>powiat radzyński</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>rycki</t>
+          <t>powiat rycki</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>świdnicki</t>
+          <t>powiat świdnicki</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>tomaszowski</t>
+          <t>powiat tomaszowski</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>włodawski</t>
+          <t>powiat włodawski</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2402,7 +2402,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>zamojski</t>
+          <t>powiat zamojski</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>m.BiałaPodlaska</t>
+          <t>miasto BiałaPodlaska</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>m.Chełm</t>
+          <t>miasto Chełm</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2480,7 +2480,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>m.Lublin</t>
+          <t>miasto Lublin</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>m.Zamość</t>
+          <t>miasto Zamość</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>gorzowski</t>
+          <t>powiat gorzowski</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>krośnieński</t>
+          <t>powiat krośnieński</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>międzyrzecki</t>
+          <t>powiat międzyrzecki</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>nowosolski</t>
+          <t>powiat nowosolski</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>słubicki</t>
+          <t>powiat słubicki</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>strzelecko-drezdenecki</t>
+          <t>powiat strzelecko-drezdenecki</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>sulęciński</t>
+          <t>powiat sulęciński</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>świebodziński</t>
+          <t>powiat świebodziński</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>zielonogórski</t>
+          <t>powiat zielonogórski</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2784,7 +2784,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>żagański</t>
+          <t>powiat żagański</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>żarski</t>
+          <t>powiat żarski</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>wschowski</t>
+          <t>powiat wschowski</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>m.GorzówWielkopolski</t>
+          <t>miasto GorzówWielkopolski</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>m.ZielonaGóra</t>
+          <t>miasto ZielonaGóra</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>bełchatowski</t>
+          <t>powiat bełchatowski</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>kutnowski</t>
+          <t>powiat kutnowski</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>łaski</t>
+          <t>powiat łaski</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>łęczycki</t>
+          <t>powiat łęczycki</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -3018,7 +3018,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>łowicki</t>
+          <t>powiat łowicki</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>łódzkiwschodni</t>
+          <t>powiat łódzkiwschodni</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -3070,7 +3070,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>opoczyński</t>
+          <t>powiat opoczyński</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>pabianicki</t>
+          <t>powiat pabianicki</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -3122,7 +3122,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>pajęczański</t>
+          <t>powiat pajęczański</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>piotrkowski</t>
+          <t>powiat piotrkowski</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>poddębicki</t>
+          <t>powiat poddębicki</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>radomszczański</t>
+          <t>powiat radomszczański</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>rawski</t>
+          <t>powiat rawski</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>sieradzki</t>
+          <t>powiat sieradzki</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>skierniewicki</t>
+          <t>powiat skierniewicki</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>tomaszowski</t>
+          <t>powiat tomaszowski</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>wieluński</t>
+          <t>powiat wieluński</t>
         </is>
       </c>
       <c r="D109" t="n">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>wieruszowski</t>
+          <t>powiat wieruszowski</t>
         </is>
       </c>
       <c r="D110" t="n">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>zduńskowolski</t>
+          <t>powiat zduńskowolski</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>zgierski</t>
+          <t>powiat zgierski</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>brzeziński</t>
+          <t>powiat brzeziński</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3434,7 +3434,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>m.Łódź</t>
+          <t>miasto Łódź</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>m.PiotrkówTrybunalski</t>
+          <t>miasto PiotrkówTrybunalski</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3482,7 +3482,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>m.Skierniewice</t>
+          <t>miasto Skierniewice</t>
         </is>
       </c>
       <c r="D116" t="n">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>bocheński</t>
+          <t>powiat bocheński</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3534,7 +3534,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>brzeski</t>
+          <t>powiat brzeski</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>chrzanowski</t>
+          <t>powiat chrzanowski</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>dąbrowski</t>
+          <t>powiat dąbrowski</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3612,7 +3612,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>gorlicki</t>
+          <t>powiat gorlicki</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>krakowski</t>
+          <t>powiat krakowski</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>limanowski</t>
+          <t>powiat limanowski</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>miechowski</t>
+          <t>powiat miechowski</t>
         </is>
       </c>
       <c r="D124" t="n">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>myślenicki</t>
+          <t>powiat myślenicki</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>nowosądecki</t>
+          <t>powiat nowosądecki</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3764,7 +3764,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>nowotarski</t>
+          <t>powiat nowotarski</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>olkuski</t>
+          <t>powiat olkuski</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3812,7 +3812,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>oświęcimski</t>
+          <t>powiat oświęcimski</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>proszowicki</t>
+          <t>powiat proszowicki</t>
         </is>
       </c>
       <c r="D130" t="n">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>suski</t>
+          <t>powiat suski</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>tarnowski</t>
+          <t>powiat tarnowski</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>tatrzański</t>
+          <t>powiat tatrzański</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>wadowicki</t>
+          <t>powiat wadowicki</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>wielicki</t>
+          <t>powiat wielicki</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3980,7 +3980,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>m.Kraków</t>
+          <t>miasto Kraków</t>
         </is>
       </c>
       <c r="D136" t="n">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>m.NowySącz</t>
+          <t>miasto NowySącz</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>m.Tarnów</t>
+          <t>miasto Tarnów</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>białobrzeski</t>
+          <t>powiat białobrzeski</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4080,7 +4080,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>ciechanowski</t>
+          <t>powiat ciechanowski</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>garwoliński</t>
+          <t>powiat garwoliński</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>gostyniński</t>
+          <t>powiat gostyniński</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -4158,7 +4158,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>grodziski</t>
+          <t>powiat grodziski</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>grójecki</t>
+          <t>powiat grójecki</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>kozienicki</t>
+          <t>powiat kozienicki</t>
         </is>
       </c>
       <c r="D145" t="n">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>legionowski</t>
+          <t>powiat legionowski</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>lipski</t>
+          <t>powiat lipski</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>łosicki</t>
+          <t>powiat łosicki</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -4310,7 +4310,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>makowski</t>
+          <t>powiat makowski</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>miński</t>
+          <t>powiat miński</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>mławski</t>
+          <t>powiat mławski</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4382,7 +4382,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>nowodworski</t>
+          <t>powiat nowodworski</t>
         </is>
       </c>
       <c r="D152" t="n">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>ostrołęcki</t>
+          <t>powiat ostrołęcki</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>ostrowski</t>
+          <t>powiat ostrowski</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>otwocki</t>
+          <t>powiat otwocki</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>piaseczyński</t>
+          <t>powiat piaseczyński</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>płocki</t>
+          <t>powiat płocki</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>płoński</t>
+          <t>powiat płoński</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4550,7 +4550,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>pruszkowski</t>
+          <t>powiat pruszkowski</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>przasnyski</t>
+          <t>powiat przasnyski</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>przysuski</t>
+          <t>powiat przysuski</t>
         </is>
       </c>
       <c r="D161" t="n">
@@ -4622,7 +4622,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>pułtuski</t>
+          <t>powiat pułtuski</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>radomski</t>
+          <t>powiat radomski</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4670,7 +4670,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>siedlecki</t>
+          <t>powiat siedlecki</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4694,7 +4694,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>sierpecki</t>
+          <t>powiat sierpecki</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>sochaczewski</t>
+          <t>powiat sochaczewski</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>sokołowski</t>
+          <t>powiat sokołowski</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>szydłowiecki</t>
+          <t>powiat szydłowiecki</t>
         </is>
       </c>
       <c r="D168" t="n">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>warszawskizachodni</t>
+          <t>powiat warszawskizachodni</t>
         </is>
       </c>
       <c r="D169" t="n">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>węgrowski</t>
+          <t>powiat węgrowski</t>
         </is>
       </c>
       <c r="D170" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>wołomiński</t>
+          <t>powiat wołomiński</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4862,7 +4862,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>wyszkowski</t>
+          <t>powiat wyszkowski</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4886,7 +4886,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>zwoleński</t>
+          <t>powiat zwoleński</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -4910,7 +4910,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>żuromiński</t>
+          <t>powiat żuromiński</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>żyrardowski</t>
+          <t>powiat żyrardowski</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>m.Ostrołęka</t>
+          <t>miasto Ostrołęka</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -4982,7 +4982,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>m.Płock</t>
+          <t>miasto Płock</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>m.Radom</t>
+          <t>miasto Radom</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -5030,7 +5030,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>m.Siedlce</t>
+          <t>miasto Siedlce</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>m.Warszawa</t>
+          <t>miasto Warszawa</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>brzeski</t>
+          <t>powiat brzeski</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -5106,7 +5106,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>głubczycki</t>
+          <t>powiat głubczycki</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>kędzierzyńsko-kozielski</t>
+          <t>powiat kędzierzyńsko-kozielski</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>kluczborski</t>
+          <t>powiat kluczborski</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5184,7 +5184,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>krapkowicki</t>
+          <t>powiat krapkowicki</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -5210,7 +5210,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>namysłowski</t>
+          <t>powiat namysłowski</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5236,7 +5236,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>nyski</t>
+          <t>powiat nyski</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5262,7 +5262,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>oleski</t>
+          <t>powiat oleski</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>opolski*</t>
+          <t>powiat opolski*</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5312,7 +5312,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>prudnicki</t>
+          <t>powiat prudnicki</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5336,7 +5336,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>strzelecki</t>
+          <t>powiat strzelecki</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>m.Opole*</t>
+          <t>miasto Opole*</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5386,7 +5386,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>bieszczadzki</t>
+          <t>powiat bieszczadzki</t>
         </is>
       </c>
       <c r="D193" t="n">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>brzozowski</t>
+          <t>powiat brzozowski</t>
         </is>
       </c>
       <c r="D194" t="n">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>dębicki</t>
+          <t>powiat dębicki</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -5464,7 +5464,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>jarosławski</t>
+          <t>powiat jarosławski</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5490,7 +5490,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>jasielski</t>
+          <t>powiat jasielski</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>kolbuszowski</t>
+          <t>powiat kolbuszowski</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5542,7 +5542,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>krośnieński</t>
+          <t>powiat krośnieński</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5568,7 +5568,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>leżajski</t>
+          <t>powiat leżajski</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5594,7 +5594,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>lubaczowski</t>
+          <t>powiat lubaczowski</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>łańcucki</t>
+          <t>powiat łańcucki</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5642,7 +5642,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>mielecki</t>
+          <t>powiat mielecki</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>niżański</t>
+          <t>powiat niżański</t>
         </is>
       </c>
       <c r="D204" t="n">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>przemyski</t>
+          <t>powiat przemyski</t>
         </is>
       </c>
       <c r="D205" t="n">
@@ -5714,7 +5714,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>przeworski</t>
+          <t>powiat przeworski</t>
         </is>
       </c>
       <c r="D206" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>ropczycko-sędziszowski</t>
+          <t>powiat ropczycko-sędziszowski</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>rzeszowski</t>
+          <t>powiat rzeszowski</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5786,7 +5786,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>sanocki</t>
+          <t>powiat sanocki</t>
         </is>
       </c>
       <c r="D209" t="n">
@@ -5810,7 +5810,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>stalowowolski</t>
+          <t>powiat stalowowolski</t>
         </is>
       </c>
       <c r="D210" t="n">
@@ -5834,7 +5834,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>strzyżowski</t>
+          <t>powiat strzyżowski</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>tarnobrzeski</t>
+          <t>powiat tarnobrzeski</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5882,7 +5882,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>leski</t>
+          <t>powiat leski</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>m.Krosno</t>
+          <t>miasto Krosno</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5930,7 +5930,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>m.Przemyśl</t>
+          <t>miasto Przemyśl</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>m.Rzeszów</t>
+          <t>miasto Rzeszów</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -5978,7 +5978,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>m.Tarnobrzeg</t>
+          <t>miasto Tarnobrzeg</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>augustowski</t>
+          <t>powiat augustowski</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>białostocki</t>
+          <t>powiat białostocki</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>bielski</t>
+          <t>powiat bielski</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6082,7 +6082,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>grajewski</t>
+          <t>powiat grajewski</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>hajnowski</t>
+          <t>powiat hajnowski</t>
         </is>
       </c>
       <c r="D222" t="n">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>kolneński</t>
+          <t>powiat kolneński</t>
         </is>
       </c>
       <c r="D223" t="n">
@@ -6160,7 +6160,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>łomżyński</t>
+          <t>powiat łomżyński</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -6186,7 +6186,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>moniecki</t>
+          <t>powiat moniecki</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>sejneński</t>
+          <t>powiat sejneński</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6236,7 +6236,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>siemiatycki</t>
+          <t>powiat siemiatycki</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6260,7 +6260,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>sokólski</t>
+          <t>powiat sokólski</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>suwalski</t>
+          <t>powiat suwalski</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>wysokomazowiecki</t>
+          <t>powiat wysokomazowiecki</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>zambrowski</t>
+          <t>powiat zambrowski</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6356,7 +6356,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>m.Białystok</t>
+          <t>miasto Białystok</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6380,7 +6380,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>m.Łomża</t>
+          <t>miasto Łomża</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6404,7 +6404,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>m.Suwałki</t>
+          <t>miasto Suwałki</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6430,7 +6430,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>bytowski</t>
+          <t>powiat bytowski</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6456,7 +6456,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>chojnicki</t>
+          <t>powiat chojnicki</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>człuchowski</t>
+          <t>powiat człuchowski</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6508,7 +6508,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>gdański</t>
+          <t>powiat gdański</t>
         </is>
       </c>
       <c r="D238" t="n">
@@ -6534,7 +6534,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>kartuski</t>
+          <t>powiat kartuski</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6560,7 +6560,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>kościerski</t>
+          <t>powiat kościerski</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6586,7 +6586,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>kwidzyński</t>
+          <t>powiat kwidzyński</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -6612,7 +6612,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>lęborski</t>
+          <t>powiat lęborski</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>malborski</t>
+          <t>powiat malborski</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>nowodworski</t>
+          <t>powiat nowodworski</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>pucki</t>
+          <t>powiat pucki</t>
         </is>
       </c>
       <c r="D245" t="n">
@@ -6710,7 +6710,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>słupski</t>
+          <t>powiat słupski</t>
         </is>
       </c>
       <c r="D246" t="n">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>starogardzki</t>
+          <t>powiat starogardzki</t>
         </is>
       </c>
       <c r="D247" t="n">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>tczewski</t>
+          <t>powiat tczewski</t>
         </is>
       </c>
       <c r="D248" t="n">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>wejherowski</t>
+          <t>powiat wejherowski</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>sztumski</t>
+          <t>powiat sztumski</t>
         </is>
       </c>
       <c r="D250" t="n">
@@ -6830,7 +6830,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>m.Gdańsk</t>
+          <t>miasto Gdańsk</t>
         </is>
       </c>
       <c r="D251" t="n">
@@ -6854,7 +6854,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>m.Gdynia</t>
+          <t>miasto Gdynia</t>
         </is>
       </c>
       <c r="D252" t="n">
@@ -6878,7 +6878,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>m.Słupsk</t>
+          <t>miasto Słupsk</t>
         </is>
       </c>
       <c r="D253" t="n">
@@ -6902,7 +6902,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>m.Sopot</t>
+          <t>miasto Sopot</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>będziński</t>
+          <t>powiat będziński</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -6954,7 +6954,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>bielski</t>
+          <t>powiat bielski</t>
         </is>
       </c>
       <c r="D256" t="n">
@@ -6980,7 +6980,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>cieszyński</t>
+          <t>powiat cieszyński</t>
         </is>
       </c>
       <c r="D257" t="n">
@@ -7006,7 +7006,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>częstochowski</t>
+          <t>powiat częstochowski</t>
         </is>
       </c>
       <c r="D258" t="n">
@@ -7032,7 +7032,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>gliwicki</t>
+          <t>powiat gliwicki</t>
         </is>
       </c>
       <c r="D259" t="n">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>kłobucki</t>
+          <t>powiat kłobucki</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>lubliniecki</t>
+          <t>powiat lubliniecki</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7110,7 +7110,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>mikołowski</t>
+          <t>powiat mikołowski</t>
         </is>
       </c>
       <c r="D262" t="n">
@@ -7136,7 +7136,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>myszkowski</t>
+          <t>powiat myszkowski</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -7160,7 +7160,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>pszczyński</t>
+          <t>powiat pszczyński</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>raciborski</t>
+          <t>powiat raciborski</t>
         </is>
       </c>
       <c r="D265" t="n">
@@ -7208,7 +7208,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>rybnicki</t>
+          <t>powiat rybnicki</t>
         </is>
       </c>
       <c r="D266" t="n">
@@ -7232,7 +7232,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>tarnogórski</t>
+          <t>powiat tarnogórski</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7256,7 +7256,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>bieruńsko-lędziński</t>
+          <t>powiat bieruńsko-lędziński</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7280,7 +7280,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>wodzisławski</t>
+          <t>powiat wodzisławski</t>
         </is>
       </c>
       <c r="D269" t="n">
@@ -7304,7 +7304,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>zawierciański</t>
+          <t>powiat zawierciański</t>
         </is>
       </c>
       <c r="D270" t="n">
@@ -7328,7 +7328,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>żywiecki</t>
+          <t>powiat żywiecki</t>
         </is>
       </c>
       <c r="D271" t="n">
@@ -7352,7 +7352,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>m.Bielsko-Biała</t>
+          <t>miasto Bielsko-Biała</t>
         </is>
       </c>
       <c r="D272" t="n">
@@ -7376,7 +7376,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>m.Bytom</t>
+          <t>miasto Bytom</t>
         </is>
       </c>
       <c r="D273" t="n">
@@ -7400,7 +7400,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>m.Chorzów</t>
+          <t>miasto Chorzów</t>
         </is>
       </c>
       <c r="D274" t="n">
@@ -7424,7 +7424,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>m.Częstochowa</t>
+          <t>miasto Częstochowa</t>
         </is>
       </c>
       <c r="D275" t="n">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>m.DąbrowaGórnicza</t>
+          <t>miasto DąbrowaGórnicza</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7472,7 +7472,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>m.Gliwice</t>
+          <t>miasto Gliwice</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7496,7 +7496,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>m.Jastrzębie-Zdrój</t>
+          <t>miasto Jastrzębie-Zdrój</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7520,7 +7520,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>m.Jaworzno</t>
+          <t>miasto Jaworzno</t>
         </is>
       </c>
       <c r="D279" t="n">
@@ -7544,7 +7544,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>m.Katowice</t>
+          <t>miasto Katowice</t>
         </is>
       </c>
       <c r="D280" t="n">
@@ -7568,7 +7568,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>m.Mysłowice</t>
+          <t>miasto Mysłowice</t>
         </is>
       </c>
       <c r="D281" t="n">
@@ -7592,7 +7592,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>m.PiekaryŚląskie</t>
+          <t>miasto PiekaryŚląskie</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7616,7 +7616,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>m.RudaŚląska</t>
+          <t>miasto RudaŚląska</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7640,7 +7640,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>m.Rybnik</t>
+          <t>miasto Rybnik</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7664,7 +7664,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>m.SiemianowiceŚląskie</t>
+          <t>miasto SiemianowiceŚląskie</t>
         </is>
       </c>
       <c r="D285" t="n">
@@ -7688,7 +7688,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>m.Sosnowiec</t>
+          <t>miasto Sosnowiec</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7712,7 +7712,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>m.Świętochłowice</t>
+          <t>miasto Świętochłowice</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -7736,7 +7736,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>m.Tychy</t>
+          <t>miasto Tychy</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7760,7 +7760,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>m.Zabrze</t>
+          <t>miasto Zabrze</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7784,7 +7784,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>m.Żory</t>
+          <t>miasto Żory</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7810,7 +7810,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>buski</t>
+          <t>powiat buski</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7836,7 +7836,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>jędrzejowski</t>
+          <t>powiat jędrzejowski</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7862,7 +7862,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>kazimierski</t>
+          <t>powiat kazimierski</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7888,7 +7888,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>kielecki</t>
+          <t>powiat kielecki</t>
         </is>
       </c>
       <c r="D294" t="n">
@@ -7914,7 +7914,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>konecki</t>
+          <t>powiat konecki</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7940,7 +7940,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>opatowski</t>
+          <t>powiat opatowski</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -7966,7 +7966,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>ostrowiecki</t>
+          <t>powiat ostrowiecki</t>
         </is>
       </c>
       <c r="D297" t="n">
@@ -7992,7 +7992,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>pińczowski</t>
+          <t>powiat pińczowski</t>
         </is>
       </c>
       <c r="D298" t="n">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>sandomierski</t>
+          <t>powiat sandomierski</t>
         </is>
       </c>
       <c r="D299" t="n">
@@ -8042,7 +8042,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>skarżyski</t>
+          <t>powiat skarżyski</t>
         </is>
       </c>
       <c r="D300" t="n">
@@ -8066,7 +8066,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>starachowicki</t>
+          <t>powiat starachowicki</t>
         </is>
       </c>
       <c r="D301" t="n">
@@ -8090,7 +8090,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>staszowski</t>
+          <t>powiat staszowski</t>
         </is>
       </c>
       <c r="D302" t="n">
@@ -8114,7 +8114,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>włoszczowski</t>
+          <t>powiat włoszczowski</t>
         </is>
       </c>
       <c r="D303" t="n">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>m.Kielce</t>
+          <t>miasto Kielce</t>
         </is>
       </c>
       <c r="D304" t="n">
@@ -8164,7 +8164,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>bartoszycki</t>
+          <t>powiat bartoszycki</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -8190,7 +8190,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>braniewski</t>
+          <t>powiat braniewski</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8216,7 +8216,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>działdowski</t>
+          <t>powiat działdowski</t>
         </is>
       </c>
       <c r="D307" t="n">
@@ -8242,7 +8242,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>elbląski</t>
+          <t>powiat elbląski</t>
         </is>
       </c>
       <c r="D308" t="n">
@@ -8268,7 +8268,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>ełcki</t>
+          <t>powiat ełcki</t>
         </is>
       </c>
       <c r="D309" t="n">
@@ -8294,7 +8294,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>giżycki</t>
+          <t>powiat giżycki</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8320,7 +8320,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>iławski</t>
+          <t>powiat iławski</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8346,7 +8346,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>kętrzyński</t>
+          <t>powiat kętrzyński</t>
         </is>
       </c>
       <c r="D312" t="n">
@@ -8372,7 +8372,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>lidzbarski</t>
+          <t>powiat lidzbarski</t>
         </is>
       </c>
       <c r="D313" t="n">
@@ -8396,7 +8396,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>mrągowski</t>
+          <t>powiat mrągowski</t>
         </is>
       </c>
       <c r="D314" t="n">
@@ -8420,7 +8420,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>nidzicki</t>
+          <t>powiat nidzicki</t>
         </is>
       </c>
       <c r="D315" t="n">
@@ -8444,7 +8444,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>nowomiejski</t>
+          <t>powiat nowomiejski</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -8468,7 +8468,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>olecki</t>
+          <t>powiat olecki</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>olsztyński</t>
+          <t>powiat olsztyński</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8516,7 +8516,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>ostródzki</t>
+          <t>powiat ostródzki</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8540,7 +8540,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>piski</t>
+          <t>powiat piski</t>
         </is>
       </c>
       <c r="D320" t="n">
@@ -8564,7 +8564,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>szczycieński</t>
+          <t>powiat szczycieński</t>
         </is>
       </c>
       <c r="D321" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>gołdapski</t>
+          <t>powiat gołdapski</t>
         </is>
       </c>
       <c r="D322" t="n">
@@ -8612,7 +8612,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>węgorzewski</t>
+          <t>powiat węgorzewski</t>
         </is>
       </c>
       <c r="D323" t="n">
@@ -8636,7 +8636,7 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>m.Elbląg</t>
+          <t>miasto Elbląg</t>
         </is>
       </c>
       <c r="D324" t="n">
@@ -8660,7 +8660,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>m.Olsztyn</t>
+          <t>miasto Olsztyn</t>
         </is>
       </c>
       <c r="D325" t="n">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>chodzieski</t>
+          <t>powiat chodzieski</t>
         </is>
       </c>
       <c r="D326" t="n">
@@ -8712,7 +8712,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>czarnkowsko-trzcianecki</t>
+          <t>powiat czarnkowsko-trzcianecki</t>
         </is>
       </c>
       <c r="D327" t="n">
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>gnieźnieński</t>
+          <t>powiat gnieźnieński</t>
         </is>
       </c>
       <c r="D328" t="n">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>gostyński</t>
+          <t>powiat gostyński</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8790,7 +8790,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>grodziski</t>
+          <t>powiat grodziski</t>
         </is>
       </c>
       <c r="D330" t="n">
@@ -8816,7 +8816,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>jarociński</t>
+          <t>powiat jarociński</t>
         </is>
       </c>
       <c r="D331" t="n">
@@ -8842,7 +8842,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>kaliski</t>
+          <t>powiat kaliski</t>
         </is>
       </c>
       <c r="D332" t="n">
@@ -8868,7 +8868,7 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>kępiński</t>
+          <t>powiat kępiński</t>
         </is>
       </c>
       <c r="D333" t="n">
@@ -8894,7 +8894,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>kolski</t>
+          <t>powiat kolski</t>
         </is>
       </c>
       <c r="D334" t="n">
@@ -8918,7 +8918,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>koniński</t>
+          <t>powiat koniński</t>
         </is>
       </c>
       <c r="D335" t="n">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>kościański</t>
+          <t>powiat kościański</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8966,7 +8966,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>krotoszyński</t>
+          <t>powiat krotoszyński</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8990,7 +8990,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>leszczyński</t>
+          <t>powiat leszczyński</t>
         </is>
       </c>
       <c r="D338" t="n">
@@ -9014,7 +9014,7 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>międzychodzki</t>
+          <t>powiat międzychodzki</t>
         </is>
       </c>
       <c r="D339" t="n">
@@ -9038,7 +9038,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>nowotomyski</t>
+          <t>powiat nowotomyski</t>
         </is>
       </c>
       <c r="D340" t="n">
@@ -9062,7 +9062,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>obornicki</t>
+          <t>powiat obornicki</t>
         </is>
       </c>
       <c r="D341" t="n">
@@ -9086,7 +9086,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>ostrowski</t>
+          <t>powiat ostrowski</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -9110,7 +9110,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>ostrzeszowski</t>
+          <t>powiat ostrzeszowski</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -9134,7 +9134,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>pilski</t>
+          <t>powiat pilski</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9158,7 +9158,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>pleszewski</t>
+          <t>powiat pleszewski</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>poznański</t>
+          <t>powiat poznański</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9206,7 +9206,7 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>rawicki</t>
+          <t>powiat rawicki</t>
         </is>
       </c>
       <c r="D347" t="n">
@@ -9230,7 +9230,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>słupecki</t>
+          <t>powiat słupecki</t>
         </is>
       </c>
       <c r="D348" t="n">
@@ -9254,7 +9254,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>szamotulski</t>
+          <t>powiat szamotulski</t>
         </is>
       </c>
       <c r="D349" t="n">
@@ -9278,7 +9278,7 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>średzki</t>
+          <t>powiat średzki</t>
         </is>
       </c>
       <c r="D350" t="n">
@@ -9302,7 +9302,7 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>śremski</t>
+          <t>powiat śremski</t>
         </is>
       </c>
       <c r="D351" t="n">
@@ -9326,7 +9326,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>turecki</t>
+          <t>powiat turecki</t>
         </is>
       </c>
       <c r="D352" t="n">
@@ -9350,7 +9350,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>wągrowiecki</t>
+          <t>powiat wągrowiecki</t>
         </is>
       </c>
       <c r="D353" t="n">
@@ -9374,7 +9374,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>wolsztyński</t>
+          <t>powiat wolsztyński</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>wrzesiński</t>
+          <t>powiat wrzesiński</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9422,7 +9422,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>złotowski</t>
+          <t>powiat złotowski</t>
         </is>
       </c>
       <c r="D356" t="n">
@@ -9446,7 +9446,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>m.Kalisz</t>
+          <t>miasto Kalisz</t>
         </is>
       </c>
       <c r="D357" t="n">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>m.Konin</t>
+          <t>miasto Konin</t>
         </is>
       </c>
       <c r="D358" t="n">
@@ -9494,7 +9494,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>m.Leszno</t>
+          <t>miasto Leszno</t>
         </is>
       </c>
       <c r="D359" t="n">
@@ -9518,7 +9518,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>m.Poznań</t>
+          <t>miasto Poznań</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9544,7 +9544,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>białogardzki</t>
+          <t>powiat białogardzki</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9570,7 +9570,7 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>choszczeński</t>
+          <t>powiat choszczeński</t>
         </is>
       </c>
       <c r="D362" t="n">
@@ -9596,7 +9596,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>drawski</t>
+          <t>powiat drawski</t>
         </is>
       </c>
       <c r="D363" t="n">
@@ -9622,7 +9622,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>goleniowski</t>
+          <t>powiat goleniowski</t>
         </is>
       </c>
       <c r="D364" t="n">
@@ -9648,7 +9648,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>gryficki</t>
+          <t>powiat gryficki</t>
         </is>
       </c>
       <c r="D365" t="n">
@@ -9674,7 +9674,7 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>gryfiński</t>
+          <t>powiat gryfiński</t>
         </is>
       </c>
       <c r="D366" t="n">
@@ -9700,7 +9700,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>kamieński</t>
+          <t>powiat kamieński</t>
         </is>
       </c>
       <c r="D367" t="n">
@@ -9726,7 +9726,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>kołobrzeski</t>
+          <t>powiat kołobrzeski</t>
         </is>
       </c>
       <c r="D368" t="n">
@@ -9752,7 +9752,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>koszaliński</t>
+          <t>powiat koszaliński</t>
         </is>
       </c>
       <c r="D369" t="n">
@@ -9776,7 +9776,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>myśliborski</t>
+          <t>powiat myśliborski</t>
         </is>
       </c>
       <c r="D370" t="n">
@@ -9800,7 +9800,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>policki</t>
+          <t>powiat policki</t>
         </is>
       </c>
       <c r="D371" t="n">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>pyrzycki</t>
+          <t>powiat pyrzycki</t>
         </is>
       </c>
       <c r="D372" t="n">
@@ -9848,7 +9848,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>sławieński</t>
+          <t>powiat sławieński</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9872,7 +9872,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>stargardzki</t>
+          <t>powiat stargardzki</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>szczecinecki</t>
+          <t>powiat szczecinecki</t>
         </is>
       </c>
       <c r="D375" t="n">
@@ -9920,7 +9920,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>świdwiński</t>
+          <t>powiat świdwiński</t>
         </is>
       </c>
       <c r="D376" t="n">
@@ -9944,7 +9944,7 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>wałecki</t>
+          <t>powiat wałecki</t>
         </is>
       </c>
       <c r="D377" t="n">
@@ -9968,7 +9968,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>łobeski</t>
+          <t>powiat łobeski</t>
         </is>
       </c>
       <c r="D378" t="n">
@@ -9992,7 +9992,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>m.Koszalin</t>
+          <t>miasto Koszalin</t>
         </is>
       </c>
       <c r="D379" t="n">
@@ -10016,7 +10016,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>m.Szczecin</t>
+          <t>miasto Szczecin</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>m.Świnoujście</t>
+          <t>miasto Świnoujście</t>
         </is>
       </c>
       <c r="D381" t="n">

</xml_diff>